<commit_message>
updated test plans with row to notify test requester after completing testing + more info on duty cycles
</commit_message>
<xml_diff>
--- a/scripts/codemagic-ci/testing/Regression-Test-Plan-Template-Android-PROD-TEST.xlsx
+++ b/scripts/codemagic-ci/testing/Regression-Test-Plan-Template-Android-PROD-TEST.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27103"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27108"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cbryant/Downloads/test_plans/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{BA3699C8-9B2C-5B45-9094-3BE167760E9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EE61E4B9-376A-4E5D-982F-7A07779ABCBD}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="13_ncr:1_{BA3699C8-9B2C-5B45-9094-3BE167760E9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{31E2A5C0-F026-43C0-9AE8-26812EDA786F}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="1620" windowWidth="38400" windowHeight="19960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t xml:space="preserve">Regression Test Plan - ${APP_VERSION} - ${BUILD_ENV}  </t>
   </si>
@@ -53,7 +53,43 @@
     <t>Build Info</t>
   </si>
   <si>
-    <t>Time and Date Testing Was Completed:</t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">Time and Date Testing Was Complete (Testing must be done between </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>6 AM and 5 PM, Mon-Fri</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>(see "services duty cycle" section on the right side of the testing sheet for more info)</t>
+    </r>
   </si>
   <si>
     <t>mm/dd/yy - 00:00 AM/PM</t>
@@ -131,6 +167,9 @@
     <t>Notification Tool (PROD-TEST)</t>
   </si>
   <si>
+    <t>Notified test requester that you have completed testing (mark this box green after you have informed the test requester that you have finished testing)</t>
+  </si>
+  <si>
     <t>Barcode Generator (Code128) - Random</t>
   </si>
   <si>
@@ -148,12 +187,18 @@
   <si>
     <t>Barcode Generator (2D) - Invalid Barcode</t>
   </si>
+  <si>
+    <t>Services Duty Cycle</t>
+  </si>
+  <si>
+    <t>Platform Duty Cycle - ESR iPaaS - UCSD Collab (atlassian.net)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="14">
+  <fonts count="17">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -243,8 +288,26 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -314,6 +377,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFE3AA00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -431,7 +500,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -478,9 +547,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -511,19 +577,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -533,17 +589,29 @@
     <xf numFmtId="0" fontId="13" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -944,12 +1012,12 @@
   <dimension ref="A1:U943"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" workbookViewId="0">
-      <selection activeCell="B3" sqref="A2:XFD3"/>
+      <selection activeCell="B3" sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="103.42578125" style="10" customWidth="1"/>
+    <col min="1" max="1" width="96.5703125" style="10" customWidth="1"/>
     <col min="2" max="2" width="28.5703125" style="4" customWidth="1"/>
     <col min="3" max="3" width="5.85546875" style="2" customWidth="1"/>
     <col min="4" max="4" width="30.7109375" style="2" customWidth="1"/>
@@ -957,8 +1025,8 @@
     <col min="6" max="16384" width="14.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="6" customFormat="1" ht="49.5">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:21" s="6" customFormat="1" ht="51.75" customHeight="1">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="14" t="s">
@@ -985,13 +1053,13 @@
       <c r="U1" s="5"/>
     </row>
     <row r="2" spans="1:21" s="6" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="22" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="12"/>
@@ -1012,18 +1080,18 @@
       <c r="T2" s="5"/>
       <c r="U2" s="5"/>
     </row>
-    <row r="3" spans="1:21" ht="15.75" customHeight="1">
-      <c r="A3" s="37" t="s">
+    <row r="3" spans="1:21" ht="31.5" customHeight="1">
+      <c r="A3" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="24" t="s">
+      <c r="C3" s="24"/>
+      <c r="D3" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="31" t="s">
+      <c r="E3" s="34" t="s">
         <v>8</v>
       </c>
       <c r="F3" s="1"/>
@@ -1044,15 +1112,15 @@
       <c r="U3" s="1"/>
     </row>
     <row r="4" spans="1:21" ht="15">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="16" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="15"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="24" t="s">
+      <c r="C4" s="24"/>
+      <c r="D4" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="30" t="s">
+      <c r="E4" s="26" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="1"/>
@@ -1073,14 +1141,14 @@
       <c r="U4" s="1"/>
     </row>
     <row r="5" spans="1:21" ht="28.5">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="25"/>
-      <c r="D5" s="24" t="s">
+      <c r="C5" s="24"/>
+      <c r="D5" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="29" t="s">
+      <c r="E5" s="35" t="s">
         <v>14</v>
       </c>
       <c r="F5" s="1"/>
@@ -1101,7 +1169,7 @@
       <c r="U5" s="1"/>
     </row>
     <row r="6" spans="1:21">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="16" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="15"/>
@@ -1128,10 +1196,10 @@
         <v>16</v>
       </c>
       <c r="C7" s="1"/>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="18"/>
+      <c r="E7" s="17"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -1154,10 +1222,10 @@
         <v>18</v>
       </c>
       <c r="C8" s="1"/>
-      <c r="D8" s="24" t="s">
+      <c r="D8" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="19"/>
+      <c r="E8" s="18"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -1180,10 +1248,10 @@
         <v>20</v>
       </c>
       <c r="C9" s="1"/>
-      <c r="D9" s="24" t="s">
+      <c r="D9" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="20"/>
+      <c r="E9" s="19"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -1206,10 +1274,10 @@
         <v>22</v>
       </c>
       <c r="C10" s="1"/>
-      <c r="D10" s="24" t="s">
+      <c r="D10" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="21"/>
+      <c r="E10" s="20"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -1232,10 +1300,10 @@
         <v>24</v>
       </c>
       <c r="C11" s="1"/>
-      <c r="D11" s="24" t="s">
+      <c r="D11" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="22"/>
+      <c r="E11" s="21"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -1283,10 +1351,10 @@
       </c>
       <c r="B13" s="9"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="18" t="s">
+      <c r="D13" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="18"/>
+      <c r="E13" s="17"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
@@ -1305,14 +1373,14 @@
       <c r="U13" s="1"/>
     </row>
     <row r="14" spans="1:21">
-      <c r="A14" s="26" t="s">
+      <c r="A14" s="25" t="s">
         <v>29</v>
       </c>
       <c r="C14" s="1"/>
-      <c r="D14" s="36" t="s">
+      <c r="D14" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="10"/>
+      <c r="E14" s="29"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
@@ -1330,12 +1398,14 @@
       <c r="T14" s="1"/>
       <c r="U14" s="1"/>
     </row>
-    <row r="15" spans="1:21">
-      <c r="A15" s="7"/>
+    <row r="15" spans="1:21" ht="28.5">
+      <c r="A15" s="36" t="s">
+        <v>31</v>
+      </c>
       <c r="B15" s="3"/>
       <c r="C15" s="1"/>
-      <c r="D15" s="33" t="s">
-        <v>31</v>
+      <c r="D15" s="28" t="s">
+        <v>32</v>
       </c>
       <c r="E15" s="10"/>
       <c r="F15" s="1"/>
@@ -1359,8 +1429,8 @@
       <c r="A16" s="7"/>
       <c r="B16" s="3"/>
       <c r="C16" s="1"/>
-      <c r="D16" s="34" t="s">
-        <v>32</v>
+      <c r="D16" s="29" t="s">
+        <v>33</v>
       </c>
       <c r="E16" s="10"/>
       <c r="F16" s="1"/>
@@ -1384,8 +1454,8 @@
       <c r="A17" s="7"/>
       <c r="B17" s="3"/>
       <c r="C17" s="1"/>
-      <c r="D17" s="33" t="s">
-        <v>33</v>
+      <c r="D17" s="28" t="s">
+        <v>34</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
@@ -1408,8 +1478,8 @@
       <c r="A18" s="7"/>
       <c r="B18" s="3"/>
       <c r="C18" s="1"/>
-      <c r="D18" s="34" t="s">
-        <v>34</v>
+      <c r="D18" s="29" t="s">
+        <v>35</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
@@ -1432,8 +1502,8 @@
       <c r="A19" s="7"/>
       <c r="B19" s="3"/>
       <c r="C19" s="1"/>
-      <c r="D19" s="33" t="s">
-        <v>35</v>
+      <c r="D19" s="28" t="s">
+        <v>36</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
@@ -1456,8 +1526,8 @@
       <c r="A20" s="7"/>
       <c r="B20" s="3"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="34" t="s">
-        <v>36</v>
+      <c r="D20" s="29" t="s">
+        <v>37</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
@@ -1480,7 +1550,10 @@
       <c r="A21" s="7"/>
       <c r="B21" s="3"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="35"/>
+      <c r="D21" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" s="17"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
@@ -1502,6 +1575,10 @@
       <c r="A22" s="7"/>
       <c r="B22" s="3"/>
       <c r="C22" s="1"/>
+      <c r="D22" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" s="29"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
@@ -22712,15 +22789,25 @@
     <hyperlink ref="D18" r:id="rId5" display="https://mobile.ucsd.edu/_tools/barcode-generator/rand_datamatrix.html" xr:uid="{97C410DD-CEBD-BB47-8BCE-8A3ECDFD22E1}"/>
     <hyperlink ref="D19" r:id="rId6" xr:uid="{B2639174-1B80-FD44-BC53-302C7826664D}"/>
     <hyperlink ref="D20" r:id="rId7" display="https://mobile.ucsd.edu/_tools/barcode-generator/custom_datamatrix.html?barcode=inv@l1d!" xr:uid="{4A5607DC-EBC6-7444-BC6B-F0310D1DC3E6}"/>
+    <hyperlink ref="D22" r:id="rId8" xr:uid="{287C25BE-5567-48BA-9AB4-9B3C4AE8C359}"/>
   </hyperlinks>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <tableParts count="1">
-    <tablePart r:id="rId8"/>
+    <tablePart r:id="rId9"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100231ACC10D748F34BAA0C20ABFA72A7EA" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5b60ada5ef74d917189c377d37311689">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a56c8121-053f-455f-842b-cd566811d075" xmlns:ns3="76f06672-c643-4888-a225-c4422b0e89ee" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f62d863a5068cb9de04048c4fc264cf7" ns2:_="" ns3:_="">
     <xsd:import namespace="a56c8121-053f-455f-842b-cd566811d075"/>
@@ -22903,15 +22990,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -22919,11 +22997,11 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3EBAD5A3-24EF-4F6A-BE26-85289F4A1E2D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9AF01965-4B53-4043-B5ED-A531E4D3A7B2}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9AF01965-4B53-4043-B5ED-A531E4D3A7B2}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3EBAD5A3-24EF-4F6A-BE26-85289F4A1E2D}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>